<commit_message>
fixed bug for stock out
fixed bug when choose sales order product the qty calculated issues for
stock out and fixed the stock in can't be deleted issue.
</commit_message>
<xml_diff>
--- a/Docs/Testing Issue List-201506.xlsx
+++ b/Docs/Testing Issue List-201506.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Zhongding\Docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="51">
   <si>
     <t>#</t>
   </si>
@@ -166,13 +171,21 @@
   <si>
     <t>出库单的产品数量验证 有问题。
 当剩余库存为780时，我将最后一个订单的出库数量改为300，系统一直提示，此订单最多只能出230。</t>
+  </si>
+  <si>
+    <t>已解决</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>已解决</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -202,6 +215,13 @@
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -254,7 +274,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -313,9 +333,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -780,11 +803,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="29.7109375" customWidth="1"/>
     <col min="3" max="3" width="78.85546875" style="1" customWidth="1"/>
@@ -793,7 +817,7 @@
     <col min="7" max="7" width="13.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -816,7 +840,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="16">
         <v>1</v>
       </c>
@@ -837,7 +861,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
         <v>2</v>
       </c>
@@ -858,7 +882,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="176.25" customHeight="1">
+    <row r="4" spans="1:7" ht="176.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
         <v>3</v>
       </c>
@@ -879,7 +903,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
         <v>4</v>
       </c>
@@ -900,7 +924,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <v>5</v>
       </c>
@@ -921,7 +945,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
         <v>6</v>
       </c>
@@ -942,7 +966,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="90">
+    <row r="8" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
         <v>7</v>
       </c>
@@ -963,7 +987,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>8</v>
       </c>
@@ -984,7 +1008,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="45">
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
         <v>9</v>
       </c>
@@ -1005,7 +1029,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="16">
         <v>10</v>
       </c>
@@ -1026,7 +1050,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="120.75" customHeight="1">
+    <row r="12" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
         <v>11</v>
       </c>
@@ -1047,7 +1071,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
         <v>12</v>
       </c>
@@ -1068,7 +1092,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="26.25" customHeight="1">
+    <row r="14" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16">
         <v>13</v>
       </c>
@@ -1089,7 +1113,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="16">
         <v>14</v>
       </c>
@@ -1110,7 +1134,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
         <v>15</v>
       </c>
@@ -1131,7 +1155,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="16">
         <v>16</v>
       </c>
@@ -1152,7 +1176,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="16">
         <v>17</v>
       </c>
@@ -1173,7 +1197,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="16">
         <v>18</v>
       </c>
@@ -1194,7 +1218,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="16">
         <v>19</v>
       </c>
@@ -1215,7 +1239,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="30">
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="16">
         <v>20</v>
       </c>
@@ -1236,7 +1260,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="30">
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
         <v>21</v>
       </c>
@@ -1257,7 +1281,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="16">
         <v>22</v>
       </c>
@@ -1267,18 +1291,20 @@
       <c r="C23" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="10" t="s">
-        <v>10</v>
+      <c r="D23" s="22" t="s">
+        <v>49</v>
       </c>
       <c r="E23" s="18">
         <v>42151</v>
       </c>
-      <c r="F23" s="11"/>
+      <c r="F23" s="18">
+        <v>42153</v>
+      </c>
       <c r="G23" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="30">
+    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="16">
         <v>23</v>
       </c>
@@ -1299,7 +1325,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="157.5" customHeight="1">
+    <row r="25" spans="1:8" ht="157.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
         <v>24</v>
       </c>
@@ -1309,18 +1335,20 @@
       <c r="C25" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="10" t="s">
-        <v>10</v>
+      <c r="D25" s="22" t="s">
+        <v>50</v>
       </c>
       <c r="E25" s="18">
         <v>42152</v>
       </c>
-      <c r="F25" s="11"/>
+      <c r="F25" s="14">
+        <v>42153</v>
+      </c>
       <c r="G25" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="153.75" customHeight="1">
+    <row r="26" spans="1:8" ht="153.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="11"/>
       <c r="C26" s="12"/>
@@ -1330,7 +1358,7 @@
       <c r="G26" s="11"/>
       <c r="H26" s="19"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="11"/>
       <c r="C27" s="12"/>
@@ -1339,7 +1367,7 @@
       <c r="F27" s="14"/>
       <c r="G27" s="11"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
       <c r="B28" s="11"/>
       <c r="C28" s="12"/>
@@ -1348,7 +1376,7 @@
       <c r="F28" s="14"/>
       <c r="G28" s="11"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
       <c r="B29" s="11"/>
       <c r="C29" s="12"/>
@@ -1357,7 +1385,7 @@
       <c r="F29" s="14"/>
       <c r="G29" s="11"/>
     </row>
-    <row r="30" spans="1:8" ht="114" customHeight="1">
+    <row r="30" spans="1:8" ht="114" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9"/>
       <c r="B30" s="11"/>
       <c r="C30" s="12"/>
@@ -1366,7 +1394,7 @@
       <c r="F30" s="14"/>
       <c r="G30" s="11"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
       <c r="B31" s="11"/>
       <c r="C31" s="12"/>
@@ -1375,7 +1403,7 @@
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
     </row>
-    <row r="32" spans="1:8" ht="237.75" customHeight="1">
+    <row r="32" spans="1:8" ht="237.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16"/>
       <c r="B32" s="11"/>
       <c r="C32" s="12"/>
@@ -1384,7 +1412,7 @@
       <c r="F32" s="11"/>
       <c r="G32" s="11"/>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
       <c r="B33" s="11"/>
       <c r="C33" s="12"/>
@@ -1393,7 +1421,7 @@
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="9"/>
       <c r="B34" s="11"/>
       <c r="C34" s="12"/>
@@ -1402,7 +1430,7 @@
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="9"/>
       <c r="B35" s="11"/>
       <c r="C35" s="12"/>
@@ -1411,7 +1439,7 @@
       <c r="F35" s="11"/>
       <c r="G35" s="11"/>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="9"/>
       <c r="B36" s="11"/>
       <c r="C36" s="12"/>
@@ -1420,7 +1448,7 @@
       <c r="F36" s="11"/>
       <c r="G36" s="11"/>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="9"/>
       <c r="B37" s="11"/>
       <c r="C37" s="12"/>
@@ -1429,7 +1457,7 @@
       <c r="F37" s="11"/>
       <c r="G37" s="11"/>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
       <c r="B38" s="11"/>
       <c r="C38" s="12"/>
@@ -1438,7 +1466,7 @@
       <c r="F38" s="11"/>
       <c r="G38" s="11"/>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="9"/>
       <c r="B39" s="11"/>
       <c r="C39" s="12"/>
@@ -1447,7 +1475,7 @@
       <c r="F39" s="11"/>
       <c r="G39" s="11"/>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
       <c r="B40" s="11"/>
       <c r="C40" s="12"/>
@@ -1456,7 +1484,7 @@
       <c r="F40" s="11"/>
       <c r="G40" s="11"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="9"/>
       <c r="B41" s="11"/>
       <c r="C41" s="12"/>
@@ -1465,7 +1493,7 @@
       <c r="F41" s="11"/>
       <c r="G41" s="11"/>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="9"/>
       <c r="B42" s="11"/>
       <c r="C42" s="12"/>
@@ -1474,7 +1502,7 @@
       <c r="F42" s="11"/>
       <c r="G42" s="11"/>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="9"/>
       <c r="B43" s="11"/>
       <c r="C43" s="12"/>
@@ -1483,7 +1511,7 @@
       <c r="F43" s="11"/>
       <c r="G43" s="11"/>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="9"/>
       <c r="B44" s="11"/>
       <c r="C44" s="12"/>
@@ -1492,7 +1520,7 @@
       <c r="F44" s="11"/>
       <c r="G44" s="11"/>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="9"/>
       <c r="B45" s="11"/>
       <c r="C45" s="12"/>
@@ -1501,7 +1529,7 @@
       <c r="F45" s="11"/>
       <c r="G45" s="11"/>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
       <c r="B46" s="11"/>
       <c r="C46" s="12"/>
@@ -1510,7 +1538,7 @@
       <c r="F46" s="11"/>
       <c r="G46" s="11"/>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="9"/>
       <c r="B47" s="11"/>
       <c r="C47" s="12"/>
@@ -1519,7 +1547,7 @@
       <c r="F47" s="11"/>
       <c r="G47" s="11"/>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="9"/>
       <c r="B48" s="11"/>
       <c r="C48" s="12"/>
@@ -1528,7 +1556,7 @@
       <c r="F48" s="11"/>
       <c r="G48" s="11"/>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="9"/>
       <c r="B49" s="11"/>
       <c r="C49" s="12"/>
@@ -1537,7 +1565,7 @@
       <c r="F49" s="11"/>
       <c r="G49" s="11"/>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="9"/>
       <c r="B50" s="11"/>
       <c r="C50" s="12"/>
@@ -1546,7 +1574,7 @@
       <c r="F50" s="11"/>
       <c r="G50" s="11"/>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="9"/>
       <c r="B51" s="11"/>
       <c r="C51" s="12"/>
@@ -1555,7 +1583,7 @@
       <c r="F51" s="11"/>
       <c r="G51" s="11"/>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="9"/>
       <c r="B52" s="11"/>
       <c r="C52" s="12"/>
@@ -1564,7 +1592,7 @@
       <c r="F52" s="11"/>
       <c r="G52" s="11"/>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="9"/>
       <c r="B53" s="11"/>
       <c r="C53" s="12"/>
@@ -1573,7 +1601,7 @@
       <c r="F53" s="11"/>
       <c r="G53" s="11"/>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="9"/>
       <c r="B54" s="11"/>
       <c r="C54" s="12"/>
@@ -1582,7 +1610,7 @@
       <c r="F54" s="11"/>
       <c r="G54" s="11"/>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="9"/>
       <c r="B55" s="11"/>
       <c r="C55" s="12"/>
@@ -1591,7 +1619,7 @@
       <c r="F55" s="11"/>
       <c r="G55" s="11"/>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="9"/>
       <c r="B56" s="11"/>
       <c r="C56" s="12"/>
@@ -1600,7 +1628,7 @@
       <c r="F56" s="11"/>
       <c r="G56" s="11"/>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="9"/>
       <c r="B57" s="13"/>
       <c r="C57" s="15"/>
@@ -1609,7 +1637,7 @@
       <c r="F57" s="13"/>
       <c r="G57" s="11"/>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="9"/>
       <c r="B58" s="13"/>
       <c r="C58" s="15"/>
@@ -1618,7 +1646,7 @@
       <c r="F58" s="13"/>
       <c r="G58" s="11"/>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="9"/>
       <c r="B59" s="13"/>
       <c r="C59" s="15"/>
@@ -1627,7 +1655,7 @@
       <c r="F59" s="13"/>
       <c r="G59" s="11"/>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B60" s="13"/>
       <c r="C60" s="15"/>
       <c r="D60" s="13"/>

</xml_diff>

<commit_message>
fixed bug for DB stock out
fixed bug for DB stock out and update issue list
</commit_message>
<xml_diff>
--- a/Docs/Testing Issue List-201506.xlsx
+++ b/Docs/Testing Issue List-201506.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="52">
   <si>
     <t>#</t>
   </si>
@@ -171,6 +171,10 @@
   <si>
     <t>出库单的产品数量验证 有问题。
 当剩余库存为780时，我将最后一个订单的出库数量改为300，系统一直提示，此订单最多只能出230。</t>
+  </si>
+  <si>
+    <t>已解决</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>已解决</t>
@@ -804,8 +808,8 @@
   <dimension ref="A1:H60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,13 +1043,15 @@
       <c r="C11" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>10</v>
+      <c r="D11" s="22" t="s">
+        <v>51</v>
       </c>
       <c r="E11" s="18">
         <v>42150</v>
       </c>
-      <c r="F11" s="11"/>
+      <c r="F11" s="18">
+        <v>42153</v>
+      </c>
       <c r="G11" s="10" t="s">
         <v>12</v>
       </c>
@@ -1060,13 +1066,15 @@
       <c r="C12" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>10</v>
+      <c r="D12" s="22" t="s">
+        <v>51</v>
       </c>
       <c r="E12" s="18">
         <v>42150</v>
       </c>
-      <c r="F12" s="11"/>
+      <c r="F12" s="18">
+        <v>42153</v>
+      </c>
       <c r="G12" s="10" t="s">
         <v>12</v>
       </c>
@@ -1123,13 +1131,15 @@
       <c r="C15" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>10</v>
+      <c r="D15" s="22" t="s">
+        <v>49</v>
       </c>
       <c r="E15" s="18">
         <v>42150</v>
       </c>
-      <c r="F15" s="11"/>
+      <c r="F15" s="18">
+        <v>42151</v>
+      </c>
       <c r="G15" s="10" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
check in issue list
</commit_message>
<xml_diff>
--- a/Docs/Testing Issue List-201506.xlsx
+++ b/Docs/Testing Issue List-201506.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="50">
   <si>
     <t>#</t>
   </si>
@@ -165,7 +165,11 @@
   </si>
   <si>
     <t>出库单的产品数量验证 有问题。
-当剩余库存为780时，我将最后一个订单的出库数量改为300，系统一直提示，此订单最多只能出230。</t>
+当剩余库存为780时，我将最后一个订单的出库数量改为300，系统一直提示，此订单最多只能出230。
+同时，选择多个订单加入到出库单中，被合并成了一个订单。</t>
+  </si>
+  <si>
+    <t>销售订单报表只应该显示如下三种状态的订单： 已审核/发货中/已完成</t>
   </si>
 </sst>
 </file>
@@ -183,6 +187,7 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="黑体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -780,8 +785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1320,14 +1325,24 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="153.75" customHeight="1">
+    <row r="26" spans="1:8">
       <c r="A26" s="9"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
+      <c r="B26" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="18">
+        <v>42152</v>
+      </c>
+      <c r="F26" s="13"/>
+      <c r="G26" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="H26" s="19"/>
     </row>
     <row r="27" spans="1:8">

</xml_diff>